<commit_message>
more excel KEY refinement
</commit_message>
<xml_diff>
--- a/modification indices KEY.xlsx
+++ b/modification indices KEY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kulas\Git\SIOP-Engagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA9D825-EA04-41D1-8C1E-B14D2F285B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B3CACA-9459-4049-A43F-DBEC9E112317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
+    <workbookView xWindow="5376" yWindow="384" windowWidth="13404" windowHeight="12216" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="24">
   <si>
     <t>item</t>
   </si>
@@ -90,7 +90,22 @@
     <t>4 &amp; 14</t>
   </si>
   <si>
-    <t>11 &amp; 12</t>
+    <t>11 or 12</t>
+  </si>
+  <si>
+    <t>33 or 34</t>
+  </si>
+  <si>
+    <t>8 &amp; 19</t>
+  </si>
+  <si>
+    <t>2 &amp; 14</t>
+  </si>
+  <si>
+    <t>7 &amp; 19</t>
+  </si>
+  <si>
+    <t>9 or 10</t>
   </si>
 </sst>
 </file>
@@ -175,13 +190,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,7 +514,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,10 +534,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="6"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
@@ -537,7 +552,7 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -551,10 +566,10 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -568,7 +583,10 @@
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -582,7 +600,10 @@
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -599,7 +620,10 @@
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="E6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -613,8 +637,8 @@
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>18</v>
+      <c r="F7" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -627,6 +651,9 @@
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="F8" s="8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
@@ -637,6 +664,9 @@
       </c>
       <c r="C9" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
constrained factor covariances (all) after reading Eid et al (Renata article). Solution does look to improve a bit.
</commit_message>
<xml_diff>
--- a/modification indices KEY.xlsx
+++ b/modification indices KEY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kulas\Git\SIOP-Engagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B3CACA-9459-4049-A43F-DBEC9E112317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A13A00-EC29-4B6F-A11C-F9BFD9A9F783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5376" yWindow="384" windowWidth="13404" windowHeight="12216" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
+    <workbookView xWindow="768" yWindow="744" windowWidth="22272" windowHeight="12216" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,7 +514,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,6 +522,8 @@
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.109375" customWidth="1"/>
     <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="26.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
refocused problem solve on item deletions and retentions as well as modification index write.csvs
</commit_message>
<xml_diff>
--- a/modification indices KEY.xlsx
+++ b/modification indices KEY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kulas\Git\SIOP-Engagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A13A00-EC29-4B6F-A11C-F9BFD9A9F783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF0A311-40C2-4BF3-89C7-E2A1FC060B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="744" windowWidth="22272" windowHeight="12216" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
+    <workbookView xWindow="8952" yWindow="648" windowWidth="13212" windowHeight="12216" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -121,7 +121,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,6 +170,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -183,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -197,6 +203,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,7 +521,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,13 +566,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="9" t="s">
@@ -984,5 +991,6 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2 and 12 work - beyond that nope
</commit_message>
<xml_diff>
--- a/modification indices KEY.xlsx
+++ b/modification indices KEY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kulas\Git\SIOP-Engagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF0A311-40C2-4BF3-89C7-E2A1FC060B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354182F2-BEA9-43F9-9D59-EF1A83CCC4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8952" yWindow="648" windowWidth="13212" windowHeight="12216" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
+    <workbookView xWindow="7536" yWindow="96" windowWidth="13212" windowHeight="12216" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="25">
   <si>
     <t>item</t>
   </si>
@@ -72,12 +72,6 @@
     <t>Delete</t>
   </si>
   <si>
-    <t>Retain</t>
-  </si>
-  <si>
-    <t>2 or 4</t>
-  </si>
-  <si>
     <t>8 &amp; 18</t>
   </si>
   <si>
@@ -90,12 +84,6 @@
     <t>4 &amp; 14</t>
   </si>
   <si>
-    <t>11 or 12</t>
-  </si>
-  <si>
-    <t>33 or 34</t>
-  </si>
-  <si>
     <t>8 &amp; 19</t>
   </si>
   <si>
@@ -105,7 +93,22 @@
     <t>7 &amp; 19</t>
   </si>
   <si>
-    <t>9 or 10</t>
+    <t>Retain (sub)</t>
+  </si>
+  <si>
+    <t>Retain (Att)</t>
+  </si>
+  <si>
+    <t>2 or 4 (2, wording)</t>
+  </si>
+  <si>
+    <t>11 or 12 (12, association with 1)</t>
+  </si>
+  <si>
+    <t>33 or 34 (33, wording)</t>
+  </si>
+  <si>
+    <t>9 or 10 (9, variance)</t>
   </si>
 </sst>
 </file>
@@ -189,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -200,10 +203,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{507738C5-E9B0-4143-B773-B9026D58D4A3}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,7 +537,7 @@
     <col min="6" max="6" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,12 +547,12 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -562,61 +566,67 @@
         <v>11</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
-        <v>2</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="7" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -630,13 +640,13 @@
         <v>7</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -647,10 +657,10 @@
         <v>8</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -661,10 +671,10 @@
         <v>8</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -675,10 +685,10 @@
         <v>8</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -689,7 +699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -700,7 +710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -711,18 +721,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -733,7 +743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -744,7 +754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
updates to SIOPpapaja and minor item deletion pending review from Dr. Kulas
</commit_message>
<xml_diff>
--- a/modification indices KEY.xlsx
+++ b/modification indices KEY.xlsx
@@ -1,40 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kulas\Git\SIOP-Engagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\SIOP-Engagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDE9505-13D1-4138-A0F8-FE5C29D3CB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C8A8E3-EF91-4288-B56B-530BB9BF62B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6936" yWindow="2040" windowWidth="12948" windowHeight="12216" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="28">
   <si>
     <t>item</t>
   </si>
@@ -112,6 +103,12 @@
   </si>
   <si>
     <t>13 deleted, 16 retained</t>
+  </si>
+  <si>
+    <t>17 or 18</t>
+  </si>
+  <si>
+    <t>17 deleted, 18 retained? Unsure if did this correctly</t>
   </si>
 </sst>
 </file>
@@ -528,7 +525,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,6 +533,7 @@
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.109375" customWidth="1"/>
     <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="110.44140625" customWidth="1"/>
     <col min="5" max="5" width="26.88671875" customWidth="1"/>
     <col min="6" max="6" width="22.88671875" customWidth="1"/>
   </cols>
@@ -676,6 +674,9 @@
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="E8" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="F8" s="8" t="s">
         <v>17</v>
       </c>
@@ -771,7 +772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -782,7 +783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -792,8 +793,11 @@
       <c r="C18" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -804,7 +808,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -815,7 +819,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -826,7 +830,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -837,7 +841,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -848,7 +852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -859,7 +863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -870,7 +874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -881,7 +885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -892,7 +896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -903,7 +907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -914,7 +918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -925,7 +929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -936,7 +940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
blacked out mod indicies key to reflect 8/6 item reduction
</commit_message>
<xml_diff>
--- a/modification indices KEY.xlsx
+++ b/modification indices KEY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\SIOP-Engagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4B27F4-B949-4713-9E31-746BD86AC81C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC7EC33-6599-4679-80D8-9886683E73D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
+    <workbookView xWindow="6180" yWindow="0" windowWidth="12960" windowHeight="8040" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -217,10 +217,10 @@
     <xf numFmtId="16" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{507738C5-E9B0-4143-B773-B9026D58D4A3}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,10 +561,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="12"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
@@ -624,13 +624,13 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -661,13 +661,13 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -712,13 +712,13 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="A10" s="11">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -779,7 +779,7 @@
       <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>31</v>
       </c>
     </row>
@@ -823,13 +823,13 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+      <c r="A19" s="11">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>8</v>
       </c>
     </row>
@@ -845,13 +845,13 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+      <c r="A21" s="11">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="B21" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>8</v>
       </c>
     </row>
@@ -900,13 +900,13 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+      <c r="A26" s="11">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="B26" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -922,13 +922,13 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
+      <c r="A28" s="11">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B28" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -944,13 +944,13 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
+      <c r="A30" s="11">
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>8</v>
       </c>
     </row>
@@ -988,13 +988,13 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
+      <c r="A34" s="11">
         <v>33</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="5" t="s">
+      <c r="B34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added column of item wordings to mod indices key
</commit_message>
<xml_diff>
--- a/modification indices KEY.xlsx
+++ b/modification indices KEY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\SIOP-Engagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC7EC33-6599-4679-80D8-9886683E73D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C452E233-3E7C-401B-8843-7BDE39F91179}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="0" windowWidth="12960" windowHeight="8040" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="68">
   <si>
     <t>item</t>
   </si>
@@ -121,16 +121,130 @@
   </si>
   <si>
     <t>test stat removing item 18 = 711</t>
+  </si>
+  <si>
+    <t>  Item_1=`Iâ€™m able to concentrate on my work without distractions.`,</t>
+  </si>
+  <si>
+    <t>  Item_2=`I have a hard time detaching mentally from my work.`,</t>
+  </si>
+  <si>
+    <t>  Item_3=`Time passes quickly while Iâ€™m working.`,</t>
+  </si>
+  <si>
+    <t>  Item_4=`I find it difficult to mentally disconnect from work.`,</t>
+  </si>
+  <si>
+    <t>  Item_5=`I enjoy thinking about work even when Iâ€™m not at work.`,</t>
+  </si>
+  <si>
+    <t>  Item_6=`Most days, I feel happiest when the workday is soon to be complete.`,</t>
+  </si>
+  <si>
+    <t>  Item_7=`I am happiest when I am immersed in a project.`,</t>
+  </si>
+  <si>
+    <t>  Item_8=`I love starting my workday.`,</t>
+  </si>
+  <si>
+    <t>  Item_9=`I devote more time than is expected of me.`,</t>
+  </si>
+  <si>
+    <t>  Item_10=`I have to be reminded to take breaks while Iâ€™m at work.`,</t>
+  </si>
+  <si>
+    <t>  Item_11=`I never miss a work deadline.`,</t>
+  </si>
+  <si>
+    <t>  Item_12=`I never allow distractions to interfere with my work.`,</t>
+  </si>
+  <si>
+    <t>  Item_13=`I devote my full attention to my work tasks throughout the day.`,</t>
+  </si>
+  <si>
+    <t>  Item_14=`Thinking about work saps my energy.`,</t>
+  </si>
+  <si>
+    <t>  Item_15=`I would rather direct my focus toward a work task than a personal task.`,</t>
+  </si>
+  <si>
+    <t>  Item_16=`Iâ€™m able to maintain good levels of energy throughout the workday.`,</t>
+  </si>
+  <si>
+    <t>  Item_17=`I enjoy spending time completing my job tasks.`,</t>
+  </si>
+  <si>
+    <t>  Item_18=`Most days I feel enthusiastic about starting my work day.`,</t>
+  </si>
+  <si>
+    <t>  Item_19=`I feel motivated to go beyond what is asked of me.`,</t>
+  </si>
+  <si>
+    <t>  Item_20=`This job drains my energy.`,</t>
+  </si>
+  <si>
+    <t>  Item_21=`When work is slow I find ways to be productive.`,</t>
+  </si>
+  <si>
+    <t>  Item_22=`I express enthusiasm for my job while at work.`,</t>
+  </si>
+  <si>
+    <t>  Item_23=`I try my best to perform well at work.`,</t>
+  </si>
+  <si>
+    <t>  Item_24=`If I notice my energy level is low, I take corrective steps to re-energize.`,</t>
+  </si>
+  <si>
+    <t>  Item_25=`I plan my future with this company.`,</t>
+  </si>
+  <si>
+    <t>  Item_26=`I believe this company cares about my career goals.`,</t>
+  </si>
+  <si>
+    <t>  Item_27=`I often think about finding another job.`,</t>
+  </si>
+  <si>
+    <t>  Item_28=`This organization challenges me to work at my full potential.`,</t>
+  </si>
+  <si>
+    <t>  Item_29=`I am proud to be a member of this organization.`,</t>
+  </si>
+  <si>
+    <t>  Item_30=`I feel supported by my supervisor when I fail at a task.`,</t>
+  </si>
+  <si>
+    <t>  Item_31=`I feel proud of my accomplishments within this organization.`,</t>
+  </si>
+  <si>
+    <t>  Item_32=`My job makes me feel like Iâ€™m part of something meaningful.`,</t>
+  </si>
+  <si>
+    <t>  Item_33=`I make valued contributions to the organization.`,</t>
+  </si>
+  <si>
+    <t>  Item_34=`I embrace challenging situations at work.`,</t>
+  </si>
+  <si>
+    <t>  Item_35=`I speak positively about this organization to others.`,</t>
+  </si>
+  <si>
+    <t>  Item_36=`This organization provides the resources necessary for me to successfully perform my job.`</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -204,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -221,6 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{507738C5-E9B0-4143-B773-B9026D58D4A3}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,12 +661,13 @@
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.109375" customWidth="1"/>
     <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="110.44140625" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="85.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="110.44140625" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,12 +677,13 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="D1"/>
+      <c r="F1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -576,17 +693,20 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -596,17 +716,20 @@
       <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -616,14 +739,17 @@
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -633,14 +759,17 @@
       <c r="C5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -650,17 +779,20 @@
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -670,14 +802,17 @@
       <c r="C7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -687,14 +822,17 @@
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="G8" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -704,14 +842,17 @@
       <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -721,8 +862,11 @@
       <c r="C10" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -732,8 +876,11 @@
       <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -743,8 +890,11 @@
       <c r="C12" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -754,8 +904,11 @@
       <c r="C13" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -766,24 +919,30 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -794,10 +953,13 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -807,8 +969,11 @@
       <c r="C17" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -819,10 +984,13 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -832,8 +1000,11 @@
       <c r="C19" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -843,8 +1014,11 @@
       <c r="C20" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>20</v>
       </c>
@@ -854,8 +1028,11 @@
       <c r="C21" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -865,8 +1042,11 @@
       <c r="C22" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -876,19 +1056,25 @@
       <c r="C23" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="11">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -898,8 +1084,11 @@
       <c r="C25" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <v>25</v>
       </c>
@@ -909,8 +1098,11 @@
       <c r="C26" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -920,8 +1112,11 @@
       <c r="C27" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>27</v>
       </c>
@@ -931,8 +1126,11 @@
       <c r="C28" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -942,8 +1140,11 @@
       <c r="C29" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>29</v>
       </c>
@@ -953,8 +1154,11 @@
       <c r="C30" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -964,8 +1168,11 @@
       <c r="C31" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -975,8 +1182,11 @@
       <c r="C32" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -986,8 +1196,11 @@
       <c r="C33" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="11">
         <v>33</v>
       </c>
@@ -997,8 +1210,11 @@
       <c r="C34" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1008,8 +1224,11 @@
       <c r="C35" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1019,8 +1238,11 @@
       <c r="C36" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1030,10 +1252,13 @@
       <c r="C37" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="D37" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Tentative final 18 items
</commit_message>
<xml_diff>
--- a/modification indices KEY.xlsx
+++ b/modification indices KEY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\SIOP-Engagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C452E233-3E7C-401B-8843-7BDE39F91179}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0536C0-2EE6-4970-896E-6CE2F36BFBC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
+    <workbookView xWindow="16500" yWindow="1860" windowWidth="12960" windowHeight="8040" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -332,10 +332,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{507738C5-E9B0-4143-B773-B9026D58D4A3}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,10 +678,10 @@
         <v>2</v>
       </c>
       <c r="D1"/>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
@@ -813,13 +813,13 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
@@ -926,13 +926,13 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="14">
+      <c r="A15" s="13">
         <v>14</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="s">
@@ -1075,13 +1075,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
+      <c r="A25" s="11">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
@@ -1159,13 +1159,13 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
+      <c r="A31" s="11">
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D31" t="s">
@@ -1243,13 +1243,13 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="5">
+      <c r="A37" s="11">
         <v>36</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D37" t="s">

</xml_diff>

<commit_message>
final key edits (attitudinal model derived)
</commit_message>
<xml_diff>
--- a/modification indices KEY.xlsx
+++ b/modification indices KEY.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\SIOP-Engagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kulas\Git\SIOP-Engagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0536C0-2EE6-4970-896E-6CE2F36BFBC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AB9541-1A5D-4A39-B748-EC5E5A002370}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16500" yWindow="1860" windowWidth="12960" windowHeight="8040" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
+    <workbookView xWindow="16500" yWindow="1860" windowWidth="12960" windowHeight="8040" activeTab="1" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Prioritizing Attitude" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="70">
   <si>
     <t>item</t>
   </si>
@@ -229,6 +230,12 @@
   </si>
   <si>
     <t>  Item_36=`This organization provides the resources necessary for me to successfully perform my job.`</t>
+  </si>
+  <si>
+    <t>Retained (Based on Attitude Associations)</t>
+  </si>
+  <si>
+    <t>Excluded</t>
   </si>
 </sst>
 </file>
@@ -250,7 +257,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,6 +312,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -318,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -336,6 +349,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{507738C5-E9B0-4143-B773-B9026D58D4A3}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1263,4 +1279,641 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24604CE8-AA76-437B-AD28-86B1EE80FBD1}">
+  <dimension ref="A1:S19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="15">
+        <v>2</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3">
+        <v>4</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7">
+        <v>6</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7">
+        <v>7</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="17">
+        <v>10</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17">
+        <v>9</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
+        <v>11</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17">
+        <v>12</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3">
+        <v>13</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="16">
+        <v>14</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7">
+        <v>18</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7">
+        <v>20</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="17">
+        <v>21</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17">
+        <v>23</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="17">
+        <v>22</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17">
+        <v>24</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3">
+        <v>25</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3">
+        <v>27</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>31</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7">
+        <v>29</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>32</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7">
+        <v>30</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="17">
+        <v>34</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17">
+        <v>33</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="17">
+        <v>35</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17">
+        <v>36</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="K1:R1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
item key update with grammar edits
</commit_message>
<xml_diff>
--- a/modification indices KEY.xlsx
+++ b/modification indices KEY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kulas\Git\SIOP-Engagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C977693-6F2C-4129-8A07-76B5F78DA7A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC25D69-BB45-4496-9D64-30F48911CE3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16500" yWindow="1860" windowWidth="12960" windowHeight="8040" firstSheet="1" activeTab="5" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
+    <workbookView xWindow="16500" yWindow="1860" windowWidth="12960" windowHeight="8040" firstSheet="2" activeTab="3" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="82">
   <si>
     <t>item</t>
   </si>
@@ -298,6 +298,18 @@
   </si>
   <si>
     <t>  Item_2=`I have a hard time detaching mentally from my work.`, [CHANGE HARD TO DIFFICULT]</t>
+  </si>
+  <si>
+    <t>I am able to concentrate on my work without getting distracted</t>
+  </si>
+  <si>
+    <t>I plan to stay with this company as my career advances</t>
+  </si>
+  <si>
+    <t>I feek motivated to go beyond what is asked of me at work</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -1407,7 +1419,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D19"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2685,7 +2697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42093553-B6C7-40A0-B0F3-9D76C93911BE}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -4073,10 +4085,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222B1B82-4AC1-4BFA-9AA2-5AB35BC453AE}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4085,129 +4097,144 @@
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>75</v>
       </c>
       <c r="B1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>77</v>
       </c>
       <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="7"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="22"/>
     </row>
-    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="28" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="22"/>
     </row>
-    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="15"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="27"/>
     </row>
-    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
         <v>74</v>
       </c>
       <c r="B12" s="27"/>
-    </row>
-    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="28" t="s">
         <v>52</v>
       </c>
       <c r="B13" s="22"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="22"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>57</v>
       </c>
       <c r="B15" s="15"/>
     </row>
-    <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
         <v>59</v>
       </c>
       <c r="B16" s="15"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>56</v>
       </c>
       <c r="B17" s="15"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>62</v>
       </c>
       <c r="B18" s="27"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>63</v>
       </c>
       <c r="B19" s="27"/>
     </row>
-    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
         <v>65</v>
       </c>
       <c r="B20" s="22"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>66</v>
       </c>

</xml_diff>